<commit_message>
Too much coding for today
need to still clean proterant_ds
</commit_message>
<xml_diff>
--- a/Data/proterant_ds.xlsx
+++ b/Data/proterant_ds.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="500"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="224">
   <si>
     <t>Liriodendron</t>
   </si>
@@ -478,9 +478,6 @@
     <t>"pollination by insects usually occurs within 2-4 weeks after bud burst" might be ambo</t>
   </si>
   <si>
-    <t>octandra</t>
-  </si>
-  <si>
     <t>Alnus</t>
   </si>
   <si>
@@ -676,9 +673,6 @@
     <t>Amelanchier</t>
   </si>
   <si>
-    <t>illinoiensis</t>
-  </si>
-  <si>
     <t>triacanthos</t>
   </si>
   <si>
@@ -689,6 +683,15 @@
   </si>
   <si>
     <t>silvic_phen_seq</t>
+  </si>
+  <si>
+    <t>pennsylvanica</t>
+  </si>
+  <si>
+    <t>illinoinensis</t>
+  </si>
+  <si>
+    <t>flava</t>
   </si>
 </sst>
 </file>
@@ -1112,8 +1115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1129,34 +1132,34 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1182,7 +1185,7 @@
         <v>39</v>
       </c>
       <c r="H2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1208,7 +1211,7 @@
         <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J3" t="s">
         <v>151</v>
@@ -1237,10 +1240,10 @@
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1266,7 +1269,7 @@
         <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1292,7 +1295,7 @@
         <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1318,7 +1321,7 @@
         <v>9</v>
       </c>
       <c r="H7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1369,7 +1372,7 @@
         <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1418,7 +1421,7 @@
         <v>39</v>
       </c>
       <c r="H11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1444,7 +1447,7 @@
         <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1455,7 +1458,7 @@
         <v>119</v>
       </c>
       <c r="C13" t="s">
-        <v>152</v>
+        <v>223</v>
       </c>
       <c r="D13" t="s">
         <v>27</v>
@@ -1470,7 +1473,7 @@
         <v>8</v>
       </c>
       <c r="H13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1519,7 +1522,7 @@
         <v>27</v>
       </c>
       <c r="H15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1527,10 +1530,10 @@
         <v>85</v>
       </c>
       <c r="B16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
@@ -1545,7 +1548,7 @@
         <v>27</v>
       </c>
       <c r="H16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1553,10 +1556,10 @@
         <v>85</v>
       </c>
       <c r="B17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D17" t="s">
         <v>16</v>
@@ -1571,7 +1574,7 @@
         <v>27</v>
       </c>
       <c r="H17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1579,7 +1582,7 @@
         <v>85</v>
       </c>
       <c r="B18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C18" t="s">
         <v>62</v>
@@ -1597,7 +1600,7 @@
         <v>27</v>
       </c>
       <c r="H18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1605,7 +1608,7 @@
         <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C19" t="s">
         <v>45</v>
@@ -1669,10 +1672,10 @@
         <v>12</v>
       </c>
       <c r="H21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1683,7 +1686,7 @@
         <v>86</v>
       </c>
       <c r="C22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D22" t="s">
         <v>27</v>
@@ -1698,10 +1701,10 @@
         <v>12</v>
       </c>
       <c r="H22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1727,7 +1730,7 @@
         <v>27</v>
       </c>
       <c r="H23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1776,10 +1779,10 @@
         <v>12</v>
       </c>
       <c r="H25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1805,7 +1808,7 @@
         <v>12</v>
       </c>
       <c r="H26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1816,7 +1819,7 @@
         <v>94</v>
       </c>
       <c r="C27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D27" t="s">
         <v>27</v>
@@ -1831,7 +1834,7 @@
         <v>12</v>
       </c>
       <c r="H27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1857,7 +1860,7 @@
         <v>27</v>
       </c>
       <c r="H28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1883,7 +1886,7 @@
         <v>27</v>
       </c>
       <c r="H29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1894,7 +1897,7 @@
         <v>94</v>
       </c>
       <c r="C30" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="D30" t="s">
         <v>27</v>
@@ -1909,7 +1912,7 @@
         <v>27</v>
       </c>
       <c r="H30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1920,7 +1923,7 @@
         <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D31" t="s">
         <v>16</v>
@@ -1935,7 +1938,7 @@
         <v>8</v>
       </c>
       <c r="H31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1946,7 +1949,7 @@
         <v>94</v>
       </c>
       <c r="C32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D32" t="s">
         <v>27</v>
@@ -1961,7 +1964,7 @@
         <v>12</v>
       </c>
       <c r="H32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1987,7 +1990,7 @@
         <v>54</v>
       </c>
       <c r="H33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1998,7 +2001,7 @@
         <v>94</v>
       </c>
       <c r="C34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D34" t="s">
         <v>27</v>
@@ -2013,7 +2016,7 @@
         <v>27</v>
       </c>
       <c r="H34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2108,7 +2111,7 @@
         <v>54</v>
       </c>
       <c r="H38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2119,7 +2122,7 @@
         <v>64</v>
       </c>
       <c r="C39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D39" t="s">
         <v>27</v>
@@ -2134,7 +2137,7 @@
         <v>12</v>
       </c>
       <c r="H39" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -2145,7 +2148,7 @@
         <v>64</v>
       </c>
       <c r="C40" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D40" t="s">
         <v>16</v>
@@ -2168,7 +2171,7 @@
         <v>38</v>
       </c>
       <c r="C41" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D41" t="s">
         <v>7</v>
@@ -2183,7 +2186,7 @@
         <v>9</v>
       </c>
       <c r="H41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2234,10 +2237,10 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
+        <v>159</v>
+      </c>
+      <c r="B44" t="s">
         <v>160</v>
-      </c>
-      <c r="B44" t="s">
-        <v>161</v>
       </c>
       <c r="C44" t="s">
         <v>19</v>
@@ -2255,7 +2258,7 @@
         <v>12</v>
       </c>
       <c r="H44" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2281,7 +2284,7 @@
         <v>12</v>
       </c>
       <c r="H45" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2307,7 +2310,7 @@
         <v>39</v>
       </c>
       <c r="H46" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2318,7 +2321,7 @@
         <v>129</v>
       </c>
       <c r="C47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D47" t="s">
         <v>27</v>
@@ -2333,7 +2336,7 @@
         <v>12</v>
       </c>
       <c r="H47" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2359,7 +2362,7 @@
         <v>39</v>
       </c>
       <c r="H48" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2370,7 +2373,7 @@
         <v>129</v>
       </c>
       <c r="C49" t="s">
-        <v>52</v>
+        <v>221</v>
       </c>
       <c r="D49" t="s">
         <v>16</v>
@@ -2385,7 +2388,7 @@
         <v>39</v>
       </c>
       <c r="H49" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2411,7 +2414,7 @@
         <v>9</v>
       </c>
       <c r="H50" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2442,10 +2445,10 @@
         <v>37</v>
       </c>
       <c r="B52" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C52" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D52" t="s">
         <v>27</v>
@@ -2460,7 +2463,7 @@
         <v>12</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I52" s="3"/>
     </row>
@@ -2489,13 +2492,13 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
+        <v>163</v>
+      </c>
+      <c r="B54" t="s">
         <v>164</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>165</v>
-      </c>
-      <c r="C54" t="s">
-        <v>166</v>
       </c>
       <c r="D54" t="s">
         <v>27</v>
@@ -2512,14 +2515,14 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
+        <v>166</v>
+      </c>
+      <c r="B55" t="s">
         <v>167</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>168</v>
       </c>
-      <c r="C55" t="s">
-        <v>169</v>
-      </c>
       <c r="D55" t="s">
         <v>27</v>
       </c>
@@ -2533,7 +2536,7 @@
         <v>12</v>
       </c>
       <c r="H55" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2582,7 +2585,7 @@
         <v>27</v>
       </c>
       <c r="H57" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2608,7 +2611,7 @@
         <v>12</v>
       </c>
       <c r="H58" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2634,7 +2637,7 @@
         <v>27</v>
       </c>
       <c r="H59" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -2660,7 +2663,7 @@
         <v>27</v>
       </c>
       <c r="H60" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -2668,10 +2671,10 @@
         <v>3</v>
       </c>
       <c r="B61" t="s">
+        <v>169</v>
+      </c>
+      <c r="C61" t="s">
         <v>170</v>
-      </c>
-      <c r="C61" t="s">
-        <v>171</v>
       </c>
       <c r="D61" t="s">
         <v>27</v>
@@ -2686,7 +2689,7 @@
         <v>54</v>
       </c>
       <c r="H61" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -2694,10 +2697,10 @@
         <v>3</v>
       </c>
       <c r="B62" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C62" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E62" t="s">
         <v>7</v>
@@ -2706,7 +2709,7 @@
         <v>27</v>
       </c>
       <c r="H62" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -2714,10 +2717,10 @@
         <v>3</v>
       </c>
       <c r="B63" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C63" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E63" t="s">
         <v>7</v>
@@ -2726,7 +2729,7 @@
         <v>27</v>
       </c>
       <c r="H63" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -2734,7 +2737,7 @@
         <v>3</v>
       </c>
       <c r="B64" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C64" t="s">
         <v>19</v>
@@ -2746,7 +2749,7 @@
         <v>27</v>
       </c>
       <c r="H64" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2772,7 +2775,7 @@
         <v>8</v>
       </c>
       <c r="H65" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2867,7 +2870,7 @@
         <v>27</v>
       </c>
       <c r="H69" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2878,7 +2881,7 @@
         <v>126</v>
       </c>
       <c r="C70" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D70" t="s">
         <v>27</v>
@@ -2893,7 +2896,7 @@
         <v>39</v>
       </c>
       <c r="H70" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2904,7 +2907,7 @@
         <v>126</v>
       </c>
       <c r="C71" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D71" t="s">
         <v>27</v>
@@ -2919,7 +2922,7 @@
         <v>8</v>
       </c>
       <c r="H71" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2945,7 +2948,7 @@
         <v>27</v>
       </c>
       <c r="H72" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2971,7 +2974,7 @@
         <v>12</v>
       </c>
       <c r="H73" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2997,7 +3000,7 @@
         <v>27</v>
       </c>
       <c r="H74" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -3023,7 +3026,7 @@
         <v>9</v>
       </c>
       <c r="H75" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -3095,7 +3098,7 @@
         <v>9</v>
       </c>
       <c r="H78" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -3121,7 +3124,7 @@
         <v>9</v>
       </c>
       <c r="H79" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -3147,7 +3150,7 @@
         <v>9</v>
       </c>
       <c r="H80" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -3173,7 +3176,7 @@
         <v>9</v>
       </c>
       <c r="H81" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -3184,7 +3187,7 @@
         <v>24</v>
       </c>
       <c r="C82" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D82" t="s">
         <v>27</v>
@@ -3199,7 +3202,7 @@
         <v>27</v>
       </c>
       <c r="H82" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -3248,7 +3251,7 @@
         <v>12</v>
       </c>
       <c r="H84" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -3274,7 +3277,7 @@
         <v>12</v>
       </c>
       <c r="H85" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -3346,7 +3349,7 @@
         <v>12</v>
       </c>
       <c r="H88" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -3372,7 +3375,7 @@
         <v>12</v>
       </c>
       <c r="H89" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -3383,7 +3386,7 @@
         <v>74</v>
       </c>
       <c r="C90" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D90" t="s">
         <v>27</v>
@@ -3398,7 +3401,7 @@
         <v>27</v>
       </c>
       <c r="H90" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -3424,7 +3427,7 @@
         <v>8</v>
       </c>
       <c r="H91" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -3473,7 +3476,7 @@
         <v>39</v>
       </c>
       <c r="H93" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -3499,7 +3502,7 @@
         <v>27</v>
       </c>
       <c r="H94" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -3525,7 +3528,7 @@
         <v>39</v>
       </c>
       <c r="H95" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -3551,7 +3554,7 @@
         <v>27</v>
       </c>
       <c r="H96" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -3600,7 +3603,7 @@
         <v>12</v>
       </c>
       <c r="H98" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -3628,7 +3631,7 @@
         <v>74</v>
       </c>
       <c r="C100" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D100" t="s">
         <v>27</v>
@@ -3643,7 +3646,7 @@
         <v>27</v>
       </c>
       <c r="H100" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="101" spans="1:10">
@@ -3669,7 +3672,7 @@
         <v>27</v>
       </c>
       <c r="H101" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="102" spans="1:10">
@@ -3680,7 +3683,7 @@
         <v>74</v>
       </c>
       <c r="C102" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D102" t="s">
         <v>27</v>
@@ -3695,7 +3698,7 @@
         <v>27</v>
       </c>
       <c r="H102" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="103" spans="1:10">
@@ -3706,7 +3709,7 @@
         <v>74</v>
       </c>
       <c r="C103" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D103" t="s">
         <v>27</v>
@@ -3721,7 +3724,7 @@
         <v>12</v>
       </c>
       <c r="H103" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="104" spans="1:10">
@@ -3732,7 +3735,7 @@
         <v>74</v>
       </c>
       <c r="C104" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D104" t="s">
         <v>27</v>
@@ -3747,7 +3750,7 @@
         <v>27</v>
       </c>
       <c r="H104" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="105" spans="1:10">
@@ -3758,7 +3761,7 @@
         <v>74</v>
       </c>
       <c r="C105" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D105" t="s">
         <v>27</v>
@@ -3773,7 +3776,7 @@
         <v>27</v>
       </c>
       <c r="H105" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="106" spans="1:10">
@@ -3784,25 +3787,25 @@
         <v>74</v>
       </c>
       <c r="C106" t="s">
+        <v>193</v>
+      </c>
+      <c r="D106" t="s">
+        <v>27</v>
+      </c>
+      <c r="E106" t="s">
+        <v>16</v>
+      </c>
+      <c r="F106" t="s">
+        <v>27</v>
+      </c>
+      <c r="G106" t="s">
         <v>194</v>
       </c>
-      <c r="D106" t="s">
-        <v>27</v>
-      </c>
-      <c r="E106" t="s">
-        <v>16</v>
-      </c>
-      <c r="F106" t="s">
-        <v>27</v>
-      </c>
-      <c r="G106" t="s">
+      <c r="H106" t="s">
+        <v>179</v>
+      </c>
+      <c r="J106" t="s">
         <v>195</v>
-      </c>
-      <c r="H106" t="s">
-        <v>180</v>
-      </c>
-      <c r="J106" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="107" spans="1:10">
@@ -3813,7 +3816,7 @@
         <v>74</v>
       </c>
       <c r="C107" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D107" t="s">
         <v>27</v>
@@ -3828,7 +3831,7 @@
         <v>12</v>
       </c>
       <c r="H107" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="108" spans="1:10">
@@ -3839,7 +3842,7 @@
         <v>74</v>
       </c>
       <c r="C108" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D108" t="s">
         <v>27</v>
@@ -3854,7 +3857,7 @@
         <v>12</v>
       </c>
       <c r="H108" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="109" spans="1:10">
@@ -3880,7 +3883,7 @@
         <v>39</v>
       </c>
       <c r="H109" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="110" spans="1:10">
@@ -3891,7 +3894,7 @@
         <v>74</v>
       </c>
       <c r="C110" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D110" t="s">
         <v>27</v>
@@ -3906,7 +3909,7 @@
         <v>12</v>
       </c>
       <c r="H110" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="111" spans="1:10">
@@ -3917,7 +3920,7 @@
         <v>74</v>
       </c>
       <c r="C111" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D111" t="s">
         <v>27</v>
@@ -3932,7 +3935,7 @@
         <v>9</v>
       </c>
       <c r="H111" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="112" spans="1:10">
@@ -3943,7 +3946,7 @@
         <v>74</v>
       </c>
       <c r="C112" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D112" t="s">
         <v>27</v>
@@ -3958,7 +3961,7 @@
         <v>12</v>
       </c>
       <c r="H112" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="113" spans="1:8">
@@ -3969,7 +3972,7 @@
         <v>74</v>
       </c>
       <c r="C113" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D113" t="s">
         <v>27</v>
@@ -3984,7 +3987,7 @@
         <v>12</v>
       </c>
       <c r="H113" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -4079,7 +4082,7 @@
         <v>8</v>
       </c>
       <c r="H117" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="118" spans="1:8">
@@ -4174,7 +4177,7 @@
         <v>39</v>
       </c>
       <c r="H121" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="122" spans="1:8">
@@ -4185,7 +4188,7 @@
         <v>11</v>
       </c>
       <c r="C122" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D122" t="s">
         <v>7</v>
@@ -4200,7 +4203,7 @@
         <v>12</v>
       </c>
       <c r="H122" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="123" spans="1:8">
@@ -4249,7 +4252,7 @@
         <v>8</v>
       </c>
       <c r="H124" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="125" spans="1:8">
@@ -4275,7 +4278,7 @@
         <v>27</v>
       </c>
       <c r="H125" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="126" spans="1:8">
@@ -4309,7 +4312,7 @@
         <v>60</v>
       </c>
       <c r="C127" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D127" t="s">
         <v>27</v>
@@ -4324,7 +4327,7 @@
         <v>9</v>
       </c>
       <c r="H127" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="128" spans="1:8">
@@ -4350,7 +4353,7 @@
         <v>9</v>
       </c>
       <c r="H128" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="129" spans="1:8">
@@ -4376,7 +4379,7 @@
         <v>9</v>
       </c>
       <c r="H129" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="130" spans="1:8">
@@ -4402,7 +4405,7 @@
         <v>9</v>
       </c>
       <c r="H130" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -4493,7 +4496,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4504,7 +4507,7 @@
         <v>145</v>
       </c>
       <c r="D3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:4">

</xml_diff>